<commit_message>
Update Notebook w/ bug for plotting EU summary
</commit_message>
<xml_diff>
--- a/RawData/BE_IGU_RawData_VPython.xlsx
+++ b/RawData/BE_IGU_RawData_VPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\02_MFA_IGU\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA80E3FE-2137-47C4-9AF2-1954A837C88C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6B0499-C2F2-42FF-A75E-4F0AD7A05131}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="600" windowWidth="18525" windowHeight="15600" activeTab="2" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
@@ -4970,7 +4970,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6034,7 +6034,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Notebook and rawdata update
</commit_message>
<xml_diff>
--- a/RawData/BE_IGU_RawData_VPython.xlsx
+++ b/RawData/BE_IGU_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\02_MFA_IGU\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FFD755-40C5-4929-854D-80C4023F5CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5853DC-8E44-4E7D-B2F0-A79DFF6F7BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="16665" windowHeight="15600" activeTab="1" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{940F02E6-5D26-4F74-996E-1951FB12C613}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{26F78B42-E424-44BA-AF5E-26A074749DFD}">
       <text>
         <r>
           <rPr>
@@ -81,11 +81,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Anon., 1958)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{299B695B-333A-460A-A8F2-9AE5A2214A15}">
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{74E54061-B8AF-4DB6-9E27-193293F73C5B}">
       <text>
         <r>
           <rPr>
@@ -94,11 +94,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{A5DBB5FC-611A-4E42-9564-E9EC2BA4A1E7}">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{B5DF2B8E-A815-46EE-8412-8A10228464A9}">
       <text>
         <r>
           <rPr>
@@ -107,11 +107,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{21AA4678-0865-4FA5-A72E-8DB4ADAAC62C}">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{8BA528D9-9C11-4FD8-B7A3-9CD002CBE26F}">
       <text>
         <r>
           <rPr>
@@ -120,11 +120,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{9D6C6068-5B0A-4AF7-95CA-F8A1631AF142}">
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{CE95B545-BDC0-4FCB-84DC-9E371DEB758E}">
       <text>
         <r>
           <rPr>
@@ -133,11 +133,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{2EB93FD8-1C2D-4CEB-9C1B-46872B2E7595}">
+    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{B59364D7-84B0-447B-B5D2-3B2B4E6B0F25}">
       <text>
         <r>
           <rPr>
@@ -146,11 +146,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{A6843698-D0E9-4171-A844-916892159473}">
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{53966744-BF41-4CC8-B348-AC3299B2CF7E}">
       <text>
         <r>
           <rPr>
@@ -159,11 +159,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{951B3F9A-1A8E-494C-ACC6-94C686FE2E0A}">
+    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{91E08B81-EA04-4BAC-88B8-D619EF8AE53E}">
       <text>
         <r>
           <rPr>
@@ -172,11 +172,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{50BB478A-BE27-4C2E-A868-1EF91684FA16}">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{B96A089B-E1E6-4F85-BD1C-6B7F6272785A}">
       <text>
         <r>
           <rPr>
@@ -185,11 +185,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{6E69AE01-93B7-4335-8309-B78781BF53A3}">
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{7E853390-C65B-4B1E-82BA-D8A4C9E23361}">
       <text>
         <r>
           <rPr>
@@ -198,11 +198,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{2C7B58A1-BDC0-4692-A025-6F4ABC339B24}">
+    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{B7A040F9-3D7B-46D5-B182-F2DBEE90C2C2}">
       <text>
         <r>
           <rPr>
@@ -211,11 +211,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{A6A4C986-2947-494C-AEC4-D08AD1F6F579}">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{B00ED96A-6E89-4F75-9ADD-A2597B97928E}">
       <text>
         <r>
           <rPr>
@@ -224,11 +224,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{AF21901A-CE1B-47B7-BB8C-9BCF503D0F3E}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{7FD4FFEC-2359-48B2-ACE9-5F3778636AD9}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Commission of the European Communities)</t>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{F0C42ADB-55C0-48CD-9FCC-76CA7BA67F8C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
         </r>
       </text>
     </comment>
@@ -278,19 +291,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{26F78B42-E424-44BA-AF5E-26A074749DFD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(Anon., 1958)</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B52" authorId="0" shapeId="0" xr:uid="{1E307675-631F-41A0-A89D-E79CDD6EFC39}">
       <text>
         <r>
@@ -1144,11 +1144,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Van de Voorde, 2016)</t>
+          <t>Average: 
+(Van de Voorde, 2016; Compagnie de Saint-Gobain, 1953)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{C73D5235-1A7D-49BA-B923-24AAD616A08A}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{E897BFD1-0DCE-4B05-A25E-C35E4A56DA2A}">
       <text>
         <r>
           <rPr>
@@ -1157,7 +1158,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Van de Voorde, 2016)</t>
+          <t>Average: 
+(Van de Voorde, 2016; Compagnie de Saint-Gobain, 1953)</t>
         </r>
       </text>
     </comment>
@@ -1165,27 +1167,16 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>jean:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-According to import and export data in 2004/2005</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>According to import and export data in 2004/2005</t>
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{687EFD71-1300-42A8-9C15-DF62C1E04FE9}">
+    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{4434DBBB-8DFD-40DF-AF85-102AB024A619}">
       <text>
         <r>
           <rPr>
@@ -2221,11 +2212,11 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,6 +2309,10 @@
       <c r="A15" s="2">
         <v>1958</v>
       </c>
+      <c r="B15" s="26">
+        <f>50</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -2728,10 +2723,10 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,10 +2818,6 @@
     <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1958</v>
-      </c>
-      <c r="B15" s="26">
-        <f>50</f>
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4176,7 +4167,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5096,13 +5087,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E0D9E8-E9D1-4F04-9EDA-8B9A7D5C3F7A}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5112,7 +5103,7 @@
     <col min="3" max="16384" width="13.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -5120,91 +5111,93 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1945</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1946</v>
       </c>
       <c r="B3" s="6">
-        <f>2*3</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <f>AVERAGE(2*3, 2*5.5)</f>
+        <v>8.5</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1947</v>
       </c>
       <c r="B4" s="53"/>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1948</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1949</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1950</v>
       </c>
       <c r="B7" s="53"/>
     </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1951</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1952</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1953</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1954</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1955</v>
       </c>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1956</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1957</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1958</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1959</v>
       </c>
@@ -5214,7 +5207,10 @@
       <c r="A17" s="2">
         <v>1960</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6">
+        <f>AVERAGE(2*3, 2*5.5)</f>
+        <v>8.5</v>
+      </c>
     </row>
     <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -5274,10 +5270,7 @@
       <c r="A27" s="2">
         <v>1970</v>
       </c>
-      <c r="B27" s="6">
-        <f>2*3</f>
-        <v>6</v>
-      </c>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -5574,8 +5567,8 @@
         <v>2019</v>
       </c>
       <c r="B76" s="5">
-        <f>2*6</f>
-        <v>12</v>
+        <f>2*5.5</f>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
The notebook is split into two parts: the first one concerns only the environmental analysis of IGU production; the second one, moved to a new notebook, concerns the stock with the prospective analysis.
</commit_message>
<xml_diff>
--- a/RawData/BE_IGU_RawData_VPython.xlsx
+++ b/RawData/BE_IGU_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\02_MFA_IGU\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5853DC-8E44-4E7D-B2F0-A79DFF6F7BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2E7E1C-3DE6-4EBF-8B66-31DAEAA62B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16665" windowHeight="15600" activeTab="1" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="1560" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="5" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
@@ -1135,7 +1135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{87EF8A9E-F82C-4199-9C4C-E69FBC2F55AF}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{5C318FAC-BCB5-462D-8D1C-99BB918B9039}">
       <text>
         <r>
           <rPr>
@@ -1149,7 +1149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{E897BFD1-0DCE-4B05-A25E-C35E4A56DA2A}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{727DC83E-897D-4B49-89D4-5DD847959BD0}">
       <text>
         <r>
           <rPr>
@@ -2212,7 +2212,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5089,11 +5089,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E0D9E8-E9D1-4F04-9EDA-8B9A7D5C3F7A}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5122,8 +5122,8 @@
         <v>1946</v>
       </c>
       <c r="B3" s="6">
-        <f>AVERAGE(2*3, 2*5.5)</f>
-        <v>8.5</v>
+        <f>AVERAGE(2*3, 2*5)</f>
+        <v>8</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -5208,8 +5208,8 @@
         <v>1960</v>
       </c>
       <c r="B17" s="6">
-        <f>AVERAGE(2*3, 2*5.5)</f>
-        <v>8.5</v>
+        <f>AVERAGE(2*3, 2*5)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update notebook. ODYM and dynamic material flow moved in 03_MFA_IGU_Stock
</commit_message>
<xml_diff>
--- a/RawData/BE_IGU_RawData_VPython.xlsx
+++ b/RawData/BE_IGU_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\02_MFA_IGU\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2E7E1C-3DE6-4EBF-8B66-31DAEAA62B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6E9C42-1DEA-4E6B-AA82-19F0AD720474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="5" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="3510" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="5" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
@@ -1121,7 +1121,7 @@
     <author>jean</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E80F3F1B-E6E1-4056-B4D5-7D3514A1C59E}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{F5AFD202-987D-4825-8FC8-AF57339CC296}">
       <text>
         <r>
           <rPr>
@@ -1130,12 +1130,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Unless otherwise indicated in a note attached to the cell, all data collected in this column comes from:
-Production industrielle: industrie du verre, Service des études et des statistiques industrielles, 1989-2004</t>
+          <t>(Piganiol, 1965)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{5C318FAC-BCB5-462D-8D1C-99BB918B9039}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{154D8EA3-B7E3-4D43-B6F6-D1C64008BB88}">
       <text>
         <r>
           <rPr>
@@ -1144,12 +1143,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Average: 
-(Van de Voorde, 2016; Compagnie de Saint-Gobain, 1953)</t>
+          <t>(Van de Voorde, 2016)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{727DC83E-897D-4B49-89D4-5DD847959BD0}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3953A7E0-4A88-47BA-8632-4D9DCC72ADA9}">
       <text>
         <r>
           <rPr>
@@ -1158,8 +1156,46 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Average: 
-(Van de Voorde, 2016; Compagnie de Saint-Gobain, 1953)</t>
+          <t>(Compagnie de Saint-Gobain, 1953)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{B8118374-8143-4C47-A54D-55FE32C8AB6E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Piganiol, 1965)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{511404C8-B546-4A0C-B20D-C5CFEC1236A6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Van de Voorde, 2016)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{FCCA2637-7093-4E61-BE02-9BCE50F697CC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Compagnie de Saint-Gobain, 1953)</t>
         </r>
       </text>
     </comment>
@@ -1176,7 +1212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{4434DBBB-8DFD-40DF-AF85-102AB024A619}">
+    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{E5930C1C-92EA-4B15-9684-03F0799ED053}">
       <text>
         <r>
           <rPr>
@@ -1185,7 +1221,63 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(Private discussion with glass industries. According to them, since 2000, average thickness is around 6mm per glass sheet)</t>
+          <t>(Leysens, 2010)
+(Hestin et al., 2016)
+(Institut für Fenstertechnik, 2015)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D62" authorId="0" shapeId="0" xr:uid="{B975DEC0-7114-4D27-83D1-AC2C76D0EF49}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Leysens, 2010)
+(Hestin et al., 2016)
+(Institut für Fenstertechnik, 2015)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{715F0533-5926-43ED-98CF-43D193901E5D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Private discussion with glass industries. According to them, since 2000, in Belgium average thickness is around 5-6mm per glass sheet)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C76" authorId="0" shapeId="0" xr:uid="{DB7AE549-FDFB-4F8F-B7A9-BF8936B88840}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Private discussion with glass industries. According to them, since 2000, in Belgium average thickness is around 5-6mm per glass sheet)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D76" authorId="0" shapeId="0" xr:uid="{E0EEE759-C8B9-4BC4-B63E-82FFD9BA7208}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Private discussion with glass industries. According to them, since 2000, in Belgium average thickness is around 5-6mm per glass sheet)</t>
         </r>
       </text>
     </comment>
@@ -1294,7 +1386,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>year</t>
   </si>
@@ -1405,6 +1497,12 @@
   </si>
   <si>
     <t>Van de Voorde, Stepanie, 2016. "Glass and Glazing in Post-War Belgium (1945-70). The Rise of Double Glazing." In: Campbell, James, et al., Further Studies in the History of Construction: the Proceedings of the Third Annual Conference of the Construction History Society. Cambridge: Construction History Society, p. 429-40.</t>
+  </si>
+  <si>
+    <t>min. thickness, mm</t>
+  </si>
+  <si>
+    <t>max. thickness, mm</t>
   </si>
 </sst>
 </file>
@@ -5090,17 +5188,18 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="53" customWidth="1"/>
-    <col min="3" max="16384" width="13.5703125" style="4"/>
+    <col min="3" max="4" width="22.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="13.5703125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5110,6 +5209,12 @@
       <c r="B1" s="16" t="s">
         <v>34</v>
       </c>
+      <c r="C1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -5121,65 +5226,96 @@
       <c r="A3" s="2">
         <v>1946</v>
       </c>
-      <c r="B3" s="6">
-        <f>AVERAGE(2*3, 2*5)</f>
-        <v>8</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1947</v>
       </c>
-      <c r="B4" s="53"/>
+      <c r="B4" s="6">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="6">
+        <f>2*5.5</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1948</v>
       </c>
       <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1949</v>
       </c>
       <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1950</v>
       </c>
       <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1951</v>
       </c>
       <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1952</v>
       </c>
       <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1953</v>
       </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1954</v>
       </c>
       <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1955</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="6">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <f>2*5.5</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -5196,286 +5332,375 @@
         <v>1958</v>
       </c>
       <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1959</v>
       </c>
       <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1960</v>
       </c>
-      <c r="B17" s="6">
-        <f>AVERAGE(2*3, 2*5)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1961</v>
       </c>
       <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1962</v>
       </c>
       <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1963</v>
       </c>
       <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1964</v>
       </c>
       <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1965</v>
       </c>
       <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1966</v>
       </c>
       <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1967</v>
       </c>
       <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1968</v>
       </c>
       <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1969</v>
       </c>
       <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1970</v>
       </c>
       <c r="B27" s="6"/>
-    </row>
-    <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1971</v>
       </c>
       <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1972</v>
       </c>
       <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1973</v>
       </c>
       <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1974</v>
       </c>
       <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1975</v>
       </c>
       <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1976</v>
       </c>
       <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1977</v>
       </c>
       <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1978</v>
       </c>
       <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1979</v>
       </c>
       <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1980</v>
       </c>
       <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1981</v>
       </c>
       <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1982</v>
       </c>
       <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1983</v>
       </c>
       <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1984</v>
       </c>
       <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1985</v>
       </c>
       <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>1986</v>
       </c>
       <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>1987</v>
       </c>
       <c r="B44" s="5"/>
-    </row>
-    <row r="45" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>1988</v>
       </c>
       <c r="B45" s="5"/>
-    </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1989</v>
       </c>
       <c r="B46" s="5"/>
-    </row>
-    <row r="47" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1990</v>
       </c>
       <c r="B47" s="5"/>
-    </row>
-    <row r="48" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1991</v>
       </c>
       <c r="B48" s="5"/>
-    </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1992</v>
       </c>
       <c r="B49" s="5"/>
-    </row>
-    <row r="50" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1993</v>
       </c>
       <c r="B50" s="5"/>
-    </row>
-    <row r="51" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1994</v>
       </c>
       <c r="B51" s="5"/>
-    </row>
-    <row r="52" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1995</v>
       </c>
       <c r="B52" s="5"/>
-    </row>
-    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1996</v>
       </c>
       <c r="B53" s="5"/>
-    </row>
-    <row r="54" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1997</v>
       </c>
       <c r="B54" s="5"/>
-    </row>
-    <row r="55" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>1998</v>
       </c>
       <c r="B55" s="5"/>
-    </row>
-    <row r="56" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1999</v>
       </c>
       <c r="B56" s="5"/>
-    </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>2000</v>
       </c>
       <c r="B57" s="5"/>
-    </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>2001</v>
       </c>
       <c r="B58" s="5"/>
     </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>2002</v>
       </c>
       <c r="B59" s="5"/>
-    </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>2003</v>
       </c>
       <c r="B60" s="5"/>
-    </row>
-    <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>2004</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>2005</v>
       </c>
@@ -5483,107 +5708,151 @@
         <f>2*5.5</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="5">
+        <f>2*4.5</f>
+        <v>9</v>
+      </c>
+      <c r="D62" s="5">
+        <f>2*6</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>2006</v>
       </c>
       <c r="B63" s="5"/>
-    </row>
-    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>2007</v>
       </c>
       <c r="B64" s="5"/>
-    </row>
-    <row r="65" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>2008</v>
       </c>
       <c r="B65" s="5"/>
-    </row>
-    <row r="66" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>2009</v>
       </c>
       <c r="B66" s="5"/>
-    </row>
-    <row r="67" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>2010</v>
       </c>
       <c r="B67" s="5"/>
-    </row>
-    <row r="68" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>2011</v>
       </c>
       <c r="B68" s="5"/>
-    </row>
-    <row r="69" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>2012</v>
       </c>
       <c r="B69" s="5"/>
-    </row>
-    <row r="70" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>2013</v>
       </c>
       <c r="B70" s="5"/>
-    </row>
-    <row r="71" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>2014</v>
       </c>
       <c r="B71" s="5"/>
-    </row>
-    <row r="72" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>2015</v>
       </c>
       <c r="B72" s="5"/>
-    </row>
-    <row r="73" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>2016</v>
       </c>
       <c r="B73" s="5"/>
-    </row>
-    <row r="74" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>2017</v>
       </c>
       <c r="B74" s="5"/>
-    </row>
-    <row r="75" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>2018</v>
       </c>
       <c r="B75" s="5"/>
-    </row>
-    <row r="76" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>2019</v>
       </c>
       <c r="B76" s="5">
-        <f>2*5.5</f>
+        <f>AVERAGE(C76:D76)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="5">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D76" s="5">
+        <f>2*6</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>2020</v>
       </c>
       <c r="B77" s="6"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First version completed. To be discussed with AS.
</commit_message>
<xml_diff>
--- a/RawData/BE_IGU_RawData_VPython.xlsx
+++ b/RawData/BE_IGU_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\02_MFA_IGU\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6E9C42-1DEA-4E6B-AA82-19F0AD720474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A87630-2EE4-44C0-BE04-8FB36921F2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="5" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
@@ -1509,12 +1509,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1661,7 +1660,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1815,9 +1814,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2821,7 +2817,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
@@ -3382,13 +3378,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FB653F-4255-4899-B7D6-3BA7509BAA32}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3838,7 +3834,7 @@
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>1992</v>
       </c>
@@ -3848,7 +3844,7 @@
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>1993</v>
       </c>
@@ -3858,14 +3854,14 @@
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>1994</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>1995</v>
       </c>
@@ -3877,7 +3873,7 @@
         <v>400.37400000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>1996</v>
       </c>
@@ -3889,7 +3885,7 @@
         <v>433.89299999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>1997</v>
       </c>
@@ -3901,7 +3897,7 @@
         <v>455.976</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>1998</v>
       </c>
@@ -3913,7 +3909,7 @@
         <v>472.53800000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>1999</v>
       </c>
@@ -3925,7 +3921,7 @@
         <v>387.34</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>2000</v>
       </c>
@@ -3938,7 +3934,7 @@
       </c>
       <c r="D57" s="23"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>2001</v>
       </c>
@@ -3951,7 +3947,7 @@
       </c>
       <c r="D58" s="23"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>2002</v>
       </c>
@@ -3964,7 +3960,7 @@
       </c>
       <c r="D59" s="23"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>2003</v>
       </c>
@@ -3975,9 +3971,9 @@
       <c r="C60" s="5">
         <v>493.12700000000001</v>
       </c>
-      <c r="D60" s="23"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="22"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>2004</v>
       </c>
@@ -3987,10 +3983,9 @@
       <c r="C61" s="5">
         <v>449.02499999999998</v>
       </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="55"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="30"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>2005</v>
       </c>
@@ -4000,10 +3995,9 @@
       <c r="C62" s="5">
         <v>699.721</v>
       </c>
-      <c r="D62" s="23"/>
-      <c r="E62" s="55"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="30"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>2006</v>
       </c>
@@ -4014,9 +4008,9 @@
       <c r="C63" s="5">
         <v>499.68599999999998</v>
       </c>
-      <c r="D63" s="23"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="22"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>2007</v>
       </c>
@@ -4027,7 +4021,7 @@
       <c r="C64" s="5">
         <v>571.02200000000005</v>
       </c>
-      <c r="D64" s="23"/>
+      <c r="D64" s="22"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
@@ -4040,7 +4034,7 @@
       <c r="C65" s="5">
         <v>599.58000000000004</v>
       </c>
-      <c r="D65" s="23"/>
+      <c r="D65" s="22"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
@@ -4266,10 +4260,10 @@
   <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4953,7 +4947,7 @@
         <v>845.51800000000003</v>
       </c>
       <c r="D63" s="22"/>
-      <c r="E63" s="30"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
@@ -5188,10 +5182,10 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5705,8 +5699,8 @@
         <v>2005</v>
       </c>
       <c r="B62" s="5">
-        <f>2*5.5</f>
-        <v>11</v>
+        <f>1/2.5*AVERAGE((AVERAGE(export!B61:B62)/AVERAGE(export!C61:C62)), (AVERAGE(import!B61:B62)/AVERAGE(import!C61:C62)))*1000</f>
+        <v>10.256147422619433</v>
       </c>
       <c r="C62" s="5">
         <f>2*4.5</f>
@@ -5891,7 +5885,7 @@
   <dimension ref="A1:AL88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>